<commit_message>
added wrong file before.. oops
</commit_message>
<xml_diff>
--- a/MSXII_PedalBoard/Project Outputs for MSXII_PedalBoard/MSXII_PedalBoard_2.1.xlsx
+++ b/MSXII_PedalBoard/Project Outputs for MSXII_PedalBoard/MSXII_PedalBoard_2.1.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4CEE339-27F8-4E90-97DE-976D7B026CDB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="75" windowWidth="15165" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="75" windowWidth="15165" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
     <sheet name="Project Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
   <si>
     <t>Title</t>
   </si>
@@ -96,13 +95,13 @@
     <t>Taiping Li</t>
   </si>
   <si>
-    <t>2018-05-21 7:16:25 PM</t>
+    <t>22/05/2018 8:08:38 PM</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>CAD</t>
+    <t>&lt;none&gt;</t>
   </si>
   <si>
     <t>17</t>
@@ -150,31 +149,19 @@
     <t>Designator</t>
   </si>
   <si>
-    <t>C1</t>
+    <t>C1, C5, C6</t>
   </si>
   <si>
     <t>C2</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
+    <t>C3, C4</t>
   </si>
   <si>
     <t>LED1</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
+    <t>P1, P2</t>
   </si>
   <si>
     <t>P3</t>
@@ -183,15 +170,12 @@
     <t>R1</t>
   </si>
   <si>
-    <t>R2</t>
+    <t>R2, R4</t>
   </si>
   <si>
     <t>R3</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -204,31 +188,28 @@
     <t>Manufacturer 1</t>
   </si>
   <si>
-    <t>Kyocera AVX</t>
-  </si>
-  <si>
-    <t>Murata</t>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
   </si>
   <si>
     <t>Taiyo Yuden</t>
   </si>
   <si>
-    <t>Wurth Electronics</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Molex</t>
+    <t>Wurth Electronics Inc.</t>
+  </si>
+  <si>
+    <t>Molex, LLC</t>
   </si>
   <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>AKM Semiconductor</t>
-  </si>
-  <si>
-    <t>Microchip</t>
+    <t>AKM Semiconductor Inc.</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
   </si>
   <si>
     <t>Texas Instruments</t>
@@ -237,7 +218,7 @@
     <t>Manufacturer Part Number 1</t>
   </si>
   <si>
-    <t>06035C-104KAT2A</t>
+    <t>06035C104KAT2A</t>
   </si>
   <si>
     <t>GCM1885C2A220JA16D</t>
@@ -249,7 +230,10 @@
     <t>150060VS75000</t>
   </si>
   <si>
-    <t>502352-0400</t>
+    <t>5600200620</t>
+  </si>
+  <si>
+    <t>5023520400</t>
   </si>
   <si>
     <t>RC0603FR-0710KL</t>
@@ -324,7 +308,7 @@
     <t>Supplier Subtotal 1</t>
   </si>
   <si>
-    <t>C:\Users\Taiping\Documents\MidnightSun\hardware\MSXII_PedalBoard\MSXII_PedalBoard.PrjPcb</t>
+    <t>C:\Users\Beshoy\Documents\midsun\hardware\MSXII_PedalBoard\MSXII_PedalBoard.PrjPcb</t>
   </si>
   <si>
     <t>None</t>
@@ -333,10 +317,10 @@
     <t>Bill of Materials For Project [MSXII_PedalBoard.PrjPcb] (No PCB Document Selected)</t>
   </si>
   <si>
-    <t>7:16:25 PM</t>
-  </si>
-  <si>
-    <t>2018-05-21</t>
+    <t>8:08:38 PM</t>
+  </si>
+  <si>
+    <t>22/05/2018</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -348,7 +332,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -594,7 +578,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3F1136-DCE1-4A70-959E-FE57A9093CD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE3F1136-DCE1-4A70-959E-FE57A9093CD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -918,38 +902,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J31"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.265625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="38.265625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.73046875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="26.19921875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.06640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.9296875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="19.46484375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="5" customWidth="1"/>
     <col min="8" max="8" width="16" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.9296875" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="5"/>
+    <col min="9" max="9" width="20" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>15</v>
       </c>
@@ -957,7 +941,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
@@ -965,7 +949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>18</v>
       </c>
@@ -973,7 +957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
@@ -986,7 +970,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>20</v>
       </c>
@@ -999,7 +983,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
@@ -1009,7 +993,7 @@
       <c r="C7" s="21"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>17</v>
       </c>
@@ -1018,7 +1002,7 @@
       </c>
       <c r="C8" s="21"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>22</v>
       </c>
@@ -1027,10 +1011,10 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>30</v>
       </c>
@@ -1038,28 +1022,28 @@
         <v>43</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>31</v>
       </c>
@@ -1067,28 +1051,28 @@
         <v>44</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G12" s="3">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12" s="8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>32</v>
       </c>
@@ -1096,28 +1080,28 @@
         <v>45</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G13" s="3">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="I13" s="8">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>33</v>
       </c>
@@ -1125,448 +1109,327 @@
         <v>46</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E15" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="F15" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="3">
-        <v>0.2</v>
+        <v>1.68</v>
       </c>
       <c r="H16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F17" s="33" t="s">
         <v>87</v>
       </c>
       <c r="G17" s="3">
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
       </c>
       <c r="I17" s="8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G18" s="3">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
       </c>
       <c r="I18" s="8">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" s="3">
-        <v>1.75</v>
+        <v>7.08</v>
       </c>
       <c r="H21" s="3">
         <v>1</v>
       </c>
       <c r="I21" s="8">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>7.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="29" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G22" s="3">
-        <v>0.13</v>
+        <v>0.43</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="8">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G23" s="3">
-        <v>0.13</v>
+        <v>4.08</v>
       </c>
       <c r="H23" s="3">
         <v>1</v>
       </c>
       <c r="I23" s="8">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1</v>
-      </c>
-      <c r="I24" s="8">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="H25" s="3">
-        <v>1</v>
-      </c>
-      <c r="I25" s="8">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="3">
-        <v>6.14</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="8">
-        <v>6.14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0.37</v>
-      </c>
-      <c r="H27" s="3">
-        <v>1</v>
-      </c>
-      <c r="I27" s="8">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G28" s="3">
-        <v>3.54</v>
-      </c>
-      <c r="H28" s="3">
-        <v>1</v>
-      </c>
-      <c r="I28" s="8">
-        <v>3.54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="3" t="s">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="12">
-        <f>SUM(I12:I28)</f>
-        <v>13.25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="15"/>
-    </row>
-    <row r="31" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="15"/>
+      <c r="I24" s="12">
+        <f>SUM(I12:I23)</f>
+        <v>18.47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1574,91 +1437,76 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" tooltip="Component" display="'Kyocera AVX" xr:uid="{4F91C639-707A-4AED-8753-EE79C4163747}"/>
-    <hyperlink ref="C13" r:id="rId2" tooltip="Component" display="'Murata" xr:uid="{E351F78C-6053-4CCD-87DB-1ADC0610C7FA}"/>
-    <hyperlink ref="C14" r:id="rId3" tooltip="Component" display="'Taiyo Yuden" xr:uid="{421147A3-BD0F-4E91-8CBB-F1CECBC90D2D}"/>
-    <hyperlink ref="C15" r:id="rId4" tooltip="Component" display="'Taiyo Yuden" xr:uid="{468DA647-693A-44F9-AB44-EB2440E85C87}"/>
-    <hyperlink ref="C16" r:id="rId5" tooltip="Component" display="'Kyocera AVX" xr:uid="{BF649ACA-F6CC-4F13-BB0A-A4EB58589134}"/>
-    <hyperlink ref="C17" r:id="rId6" tooltip="Component" display="'Kyocera AVX" xr:uid="{D1123EC6-D9B8-42E2-AA21-FD6BD6B3B68C}"/>
-    <hyperlink ref="C18" r:id="rId7" tooltip="Component" display="'Wurth Electronics" xr:uid="{ADD759C4-B9D3-4EE3-84AD-7F112CC41202}"/>
-    <hyperlink ref="C19" tooltip="Component" display="'" xr:uid="{90C3E587-6EB4-433B-B6E1-5D44A6B993DA}"/>
-    <hyperlink ref="C20" tooltip="Component" display="'" xr:uid="{4E0256ED-1A71-451F-B2BA-D9EA532AA0E3}"/>
-    <hyperlink ref="C21" r:id="rId8" tooltip="Component" display="'Molex" xr:uid="{564EEB5A-A0C6-471E-983E-BC5873EB8EBD}"/>
-    <hyperlink ref="C22" r:id="rId9" tooltip="Component" display="'Yageo" xr:uid="{19E123F7-D560-40B6-A7F7-41F705802466}"/>
-    <hyperlink ref="C23" r:id="rId10" tooltip="Component" display="'Yageo" xr:uid="{8D97E2E5-6499-4583-94A9-55367FF8FDF4}"/>
-    <hyperlink ref="C24" r:id="rId11" tooltip="Component" display="'Yageo" xr:uid="{5AD16909-337F-44C3-B4B1-93E52AD3A3CB}"/>
-    <hyperlink ref="C25" r:id="rId12" tooltip="Component" display="'Yageo" xr:uid="{9641DAD3-5774-4EB9-AFF6-66613726F9E6}"/>
-    <hyperlink ref="C26" r:id="rId13" tooltip="Component" display="'AKM Semiconductor" xr:uid="{3FE92F47-F000-466B-8783-6ADC8F2DE405}"/>
-    <hyperlink ref="C27" r:id="rId14" tooltip="Component" display="'Microchip" xr:uid="{B1DB8C05-6D07-4D81-8C38-FA393BC9C780}"/>
-    <hyperlink ref="C28" r:id="rId15" tooltip="Component" display="'Texas Instruments" xr:uid="{2F22EE9A-A8A0-4292-9DAC-C6CB05F36926}"/>
-    <hyperlink ref="D12" r:id="rId16" tooltip="Manufacturer" display="'06035C-104KAT2A" xr:uid="{4C39E476-802C-4EAF-983E-24D2430ED8DA}"/>
-    <hyperlink ref="D13" r:id="rId17" tooltip="Manufacturer" display="'GCM1885C2A220JA16D" xr:uid="{CAF78F09-164B-4811-9252-11FE54A7E4EB}"/>
-    <hyperlink ref="D14" r:id="rId18" tooltip="Manufacturer" display="'UMK107AB7105KA-T" xr:uid="{A37BC216-8779-4A10-A185-BA6A21E0E51E}"/>
-    <hyperlink ref="D15" r:id="rId19" tooltip="Manufacturer" display="'UMK107AB7105KA-T" xr:uid="{3376D692-D74A-45DC-9E46-E9B1E6454874}"/>
-    <hyperlink ref="D16" r:id="rId20" tooltip="Manufacturer" display="'06035C-104KAT2A" xr:uid="{831C18B7-A776-4426-8AD9-F29F23BB6A0C}"/>
-    <hyperlink ref="D17" r:id="rId21" tooltip="Manufacturer" display="'06035C-104KAT2A" xr:uid="{FD2E11AC-3A2E-460C-8B20-CADAE74BC722}"/>
-    <hyperlink ref="D18" r:id="rId22" tooltip="Manufacturer" display="'150060VS75000" xr:uid="{9810BF92-C627-4BF7-9A2B-4F5C10095BEF}"/>
-    <hyperlink ref="D19" tooltip="Manufacturer" display="'" xr:uid="{2B507230-74C9-4E76-A617-41A9D748012D}"/>
-    <hyperlink ref="D20" tooltip="Manufacturer" display="'" xr:uid="{7ACF2B89-4564-41FD-AF0B-06C47165B375}"/>
-    <hyperlink ref="D21" r:id="rId23" tooltip="Manufacturer" display="'502352-0400" xr:uid="{2405570F-A92D-45E5-B9CA-BC7BCD533192}"/>
-    <hyperlink ref="D22" r:id="rId24" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{F6C14549-46D8-43BC-938C-2789431C0A80}"/>
-    <hyperlink ref="D23" r:id="rId25" tooltip="Manufacturer" display="'RC0603FR-07100RL" xr:uid="{0D216752-F830-4754-AE03-432CBBC683D7}"/>
-    <hyperlink ref="D24" r:id="rId26" tooltip="Manufacturer" display="'RC0603JR-07510RL" xr:uid="{E68180C8-B35A-4795-8286-11546B4FAAE5}"/>
-    <hyperlink ref="D25" r:id="rId27" tooltip="Manufacturer" display="'RC0603FR-07100RL" xr:uid="{E2E4C80D-CA13-440A-A702-F236BB4773F6}"/>
-    <hyperlink ref="D26" r:id="rId28" tooltip="Manufacturer" display="'EM3242" xr:uid="{0C250368-328A-4988-A3FE-FB4098A06D59}"/>
-    <hyperlink ref="D27" r:id="rId29" tooltip="Manufacturer" display="'MIC94310-PYMT-TR" xr:uid="{892424B4-93AF-4DB9-BCA8-D79E371BCDBE}"/>
-    <hyperlink ref="D28" r:id="rId30" tooltip="Manufacturer" display="'ADS1015IDGSR" xr:uid="{A1313D3D-7C5C-46B5-924C-F9CA25119133}"/>
-    <hyperlink ref="F12" r:id="rId31" tooltip="Supplier" display="'478-5052-1-ND" xr:uid="{B79D9855-E57B-4992-B210-3743A1A48F1E}"/>
-    <hyperlink ref="F13" r:id="rId32" tooltip="Supplier" display="'490-4942-1-ND" xr:uid="{C8B25414-0342-4CD2-8375-EB8CCC229B23}"/>
-    <hyperlink ref="F14" r:id="rId33" tooltip="Supplier" display="'587-3247-1-ND" xr:uid="{DF7C85B5-EFCD-471E-AD87-52A330525C2B}"/>
-    <hyperlink ref="F15" r:id="rId34" tooltip="Supplier" display="'587-3247-1-ND" xr:uid="{C1EC9142-6E6D-4EC1-BDEA-1D4C2CA32B93}"/>
-    <hyperlink ref="F16" r:id="rId35" tooltip="Supplier" display="'478-5052-1-ND" xr:uid="{B31C548F-D44B-4A28-93A8-2E9A8F2D76ED}"/>
-    <hyperlink ref="F17" r:id="rId36" tooltip="Supplier" display="'478-5052-1-ND" xr:uid="{D38CDCE7-4561-4378-B9A7-1CB65183B635}"/>
-    <hyperlink ref="F18" r:id="rId37" tooltip="Supplier" display="'732-4980-1-ND" xr:uid="{2F765894-615F-4736-BF87-258A729A9449}"/>
-    <hyperlink ref="F19" tooltip="Supplier" display="'WM10866CT-ND" xr:uid="{67A45B1B-BF36-43AD-82DA-FF0B49ACBB8E}"/>
-    <hyperlink ref="F20" tooltip="Supplier" display="'WM10866CT-ND" xr:uid="{E862FFD7-4CFE-42FF-8A4A-68345BE0D5F4}"/>
-    <hyperlink ref="F21" r:id="rId38" tooltip="Supplier" display="'WM7171CT-ND" xr:uid="{1F82BC92-61B5-4C42-9BDB-F356E447CC56}"/>
-    <hyperlink ref="F22" r:id="rId39" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{F19791A6-5049-46A9-9C38-1159D92B5449}"/>
-    <hyperlink ref="F23" r:id="rId40" tooltip="Supplier" display="'311-100HRCT-ND" xr:uid="{6D4A4383-8D17-49CD-9A9B-EE329982C92E}"/>
-    <hyperlink ref="F24" r:id="rId41" tooltip="Supplier" display="'311-510GRCT-ND" xr:uid="{79E2B9B1-A055-46BC-91D9-A3557A88ED0B}"/>
-    <hyperlink ref="F25" r:id="rId42" tooltip="Supplier" display="'311-100HRCT-ND" xr:uid="{1936EDB0-801F-4377-BCAE-A4394BA963EE}"/>
-    <hyperlink ref="F26" r:id="rId43" tooltip="Supplier" display="'974-1044-1-ND" xr:uid="{3F7BE53D-7B0D-419D-B61D-F3D0DF9914FA}"/>
-    <hyperlink ref="F27" r:id="rId44" tooltip="Supplier" display="'576-4761-1-ND" xr:uid="{208C7542-E1E3-4C3B-897F-B15FA4FDB429}"/>
-    <hyperlink ref="F28" r:id="rId45" tooltip="Supplier" display="'296-41185-1-ND" xr:uid="{37CDCF70-283F-459A-9DBE-C2367A69E76B}"/>
+    <hyperlink ref="C12" r:id="rId1" tooltip="Component" display="'AVX Corporation"/>
+    <hyperlink ref="C13" r:id="rId2" tooltip="Component" display="'Murata Electronics North America"/>
+    <hyperlink ref="C14" r:id="rId3" tooltip="Component" display="'Taiyo Yuden"/>
+    <hyperlink ref="C15" r:id="rId4" tooltip="Component" display="'Wurth Electronics Inc."/>
+    <hyperlink ref="C16" r:id="rId5" tooltip="Component" display="'Molex, LLC"/>
+    <hyperlink ref="C17" r:id="rId6" tooltip="Component" display="'Molex, LLC"/>
+    <hyperlink ref="C18" r:id="rId7" tooltip="Component" display="'Yageo"/>
+    <hyperlink ref="C19" r:id="rId8" tooltip="Component" display="'Yageo"/>
+    <hyperlink ref="C20" r:id="rId9" tooltip="Component" display="'Yageo"/>
+    <hyperlink ref="C21" r:id="rId10" tooltip="Component" display="'AKM Semiconductor Inc."/>
+    <hyperlink ref="C22" r:id="rId11" tooltip="Component" display="'Microchip Technology"/>
+    <hyperlink ref="C23" r:id="rId12" tooltip="Component" display="'Texas Instruments"/>
+    <hyperlink ref="D12" r:id="rId13" tooltip="Manufacturer" display="'06035C104KAT2A"/>
+    <hyperlink ref="D13" r:id="rId14" tooltip="Manufacturer" display="'GCM1885C2A220JA16D"/>
+    <hyperlink ref="D14" r:id="rId15" tooltip="Manufacturer" display="'UMK107AB7105KA-T"/>
+    <hyperlink ref="D15" r:id="rId16" tooltip="Manufacturer" display="'150060VS75000"/>
+    <hyperlink ref="D16" r:id="rId17" tooltip="Manufacturer" display="'5600200620"/>
+    <hyperlink ref="D17" r:id="rId18" tooltip="Manufacturer" display="'5023520400"/>
+    <hyperlink ref="D18" r:id="rId19" tooltip="Manufacturer" display="'RC0603FR-0710KL"/>
+    <hyperlink ref="D19" r:id="rId20" tooltip="Manufacturer" display="'RC0603FR-07100RL"/>
+    <hyperlink ref="D20" r:id="rId21" tooltip="Manufacturer" display="'RC0603JR-07510RL"/>
+    <hyperlink ref="D21" r:id="rId22" tooltip="Manufacturer" display="'EM3242"/>
+    <hyperlink ref="D22" r:id="rId23" tooltip="Manufacturer" display="'MIC94310-PYMT-TR"/>
+    <hyperlink ref="D23" r:id="rId24" tooltip="Manufacturer" display="'ADS1015IDGSR"/>
+    <hyperlink ref="F12" r:id="rId25" tooltip="Supplier" display="'478-5052-1-ND"/>
+    <hyperlink ref="F13" r:id="rId26" tooltip="Supplier" display="'490-4942-1-ND"/>
+    <hyperlink ref="F14" r:id="rId27" tooltip="Supplier" display="'587-3247-1-ND"/>
+    <hyperlink ref="F15" r:id="rId28" tooltip="Supplier" display="'732-4980-1-ND"/>
+    <hyperlink ref="F16" r:id="rId29" tooltip="Supplier" display="'WM10866CT-ND"/>
+    <hyperlink ref="F17" r:id="rId30" tooltip="Supplier" display="'WM7171CT-ND"/>
+    <hyperlink ref="F18" r:id="rId31" tooltip="Supplier" display="'311-10.0KHRCT-ND"/>
+    <hyperlink ref="F19" r:id="rId32" tooltip="Supplier" display="'311-100HRCT-ND"/>
+    <hyperlink ref="F20" r:id="rId33" tooltip="Supplier" display="'311-510GRCT-ND"/>
+    <hyperlink ref="F21" r:id="rId34" tooltip="Supplier" display="'974-1044-1-ND"/>
+    <hyperlink ref="F22" r:id="rId35" tooltip="Supplier" display="'576-4761-1-ND"/>
+    <hyperlink ref="F23" r:id="rId36" tooltip="Supplier" display="'296-41185-1-ND"/>
   </hyperlinks>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId37"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;BAltium Limited Confidential&amp;B&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId47"/>
+  <drawing r:id="rId38"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="A1:IV65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.265625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="108.59765625" style="17" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="30.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="108.5703125" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
@@ -1666,15 +1514,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
@@ -1682,23 +1530,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
@@ -1706,23 +1554,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>10</v>
       </c>
@@ -1730,7 +1578,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
@@ -1738,23 +1586,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
HW-82 Pedal Board Rev 3 (#74)
* Changing some PCB spacing

* update steering interface connectors

* Modified pedal board with RC filtering

* Modified schematic with externarl adc

* renumbered components on analog inputs schdoc

* Added pullup resistors to I2C ouputs

* HW-82
- Updated library from HW-83 Steering Wheel Interface CAN
- Updated op-amps to correct designators

* Updated with ADC sheet

* Schematic update with changes from updated lib

* Routed and added components to PCB

* Added text and polygon pours

* Finished labelling - ready for print

* Fix the dual op-amps IC footprint and minor tweaks
- Update the footprint library
- Re-route traces around the op-amps for clearance
- Add the controller board to check clearance

* Added test points

* Fix the IC footprint

* Generated output files

* Updated libraries from master
</commit_message>
<xml_diff>
--- a/MSXII_PedalBoard/Project Outputs for MSXII_PedalBoard/MSXII_PedalBoard_2.1.xlsx
+++ b/MSXII_PedalBoard/Project Outputs for MSXII_PedalBoard/MSXII_PedalBoard_2.1.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F53BA7E3-5858-422B-94A7-696FCBD04C1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="75" windowWidth="15165" windowHeight="8820"/>
+    <workbookView xWindow="-30" yWindow="75" windowWidth="15165" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
     <sheet name="Project Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
   <si>
     <t>Title</t>
   </si>
@@ -95,7 +104,7 @@
     <t>Taiping Li</t>
   </si>
   <si>
-    <t>22/05/2018 8:08:38 PM</t>
+    <t>2019-01-18 7:44:58 PM</t>
   </si>
   <si>
     <t>1</t>
@@ -104,124 +113,154 @@
     <t>&lt;none&gt;</t>
   </si>
   <si>
-    <t>17</t>
+    <t>41</t>
   </si>
   <si>
     <t>LibRef</t>
   </si>
   <si>
+    <t>CAP CER 10nF 50V 5% X7R 0603</t>
+  </si>
+  <si>
     <t>CAP CER 0.1UF 50V 10% X7R 0603</t>
   </si>
   <si>
-    <t>CAP CER 22PF 100V 5% NP0 0603</t>
-  </si>
-  <si>
     <t>CAP CER 1UF 50V 10% X7R 0603</t>
   </si>
   <si>
     <t>LED GREEN CLEAR 2V 0603</t>
   </si>
   <si>
+    <t>CONN 2POS ULTRA-FIT 0.138"</t>
+  </si>
+  <si>
+    <t>CONN 2POS DURA-CLIK 0.079" VERT</t>
+  </si>
+  <si>
     <t>CONN 6POS DURA-CLIK 0.079"</t>
   </si>
   <si>
-    <t>CONN 4POS DURA-CLIK RIGHT ANGLE 0.079"</t>
+    <t>CONN 50POS Bergstak Plug 0.02"</t>
+  </si>
+  <si>
+    <t>CONN 4POS DURA-CLIK 0.079"</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1% 1/10W 0603</t>
   </si>
   <si>
     <t>RES 10K OHM 1% 1/10W 0603</t>
   </si>
   <si>
+    <t>RES SMD 15K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
     <t>RES 100 OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES 510 OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>IC SENSOR ROTATIONAL ANGLE 360DEG SOP6</t>
+    <t>IC OP AMP DUAL GP RR 10MHZ 8-VSSOP</t>
+  </si>
+  <si>
+    <t>IC ADC 12-BIT VSSOP-10</t>
   </si>
   <si>
     <t>IC REG LDO 3V 0.2A 4-TDFN</t>
   </si>
   <si>
-    <t>IC ADC 12-BIT VSSOP-10</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
-    <t>C1, C5, C6</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3, C4</t>
+    <t>C4, C5, C7, C8, C10, C11, C12, C14, C16, C18</t>
+  </si>
+  <si>
+    <t>C6, C9, C13, C17, C19</t>
+  </si>
+  <si>
+    <t>C20, C21</t>
   </si>
   <si>
     <t>LED1</t>
   </si>
   <si>
-    <t>P1, P2</t>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
   </si>
   <si>
     <t>P3</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2, R4</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>U3</t>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4</t>
+  </si>
+  <si>
+    <t>R8, R15</t>
+  </si>
+  <si>
+    <t>R9, R11, R13, R16</t>
+  </si>
+  <si>
+    <t>R10, R12, R14, R17</t>
+  </si>
+  <si>
+    <t>U1, U2</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U5</t>
   </si>
   <si>
     <t>Manufacturer 1</t>
   </si>
   <si>
-    <t>AVX Corporation</t>
-  </si>
-  <si>
-    <t>Murata Electronics North America</t>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>Kyocera AVX</t>
   </si>
   <si>
     <t>Taiyo Yuden</t>
   </si>
   <si>
-    <t>Wurth Electronics Inc.</t>
-  </si>
-  <si>
-    <t>Molex, LLC</t>
+    <t>Wurth Electronics</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
   </si>
   <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>AKM Semiconductor Inc.</t>
-  </si>
-  <si>
-    <t>Microchip Technology</t>
+    <t>Yageo Phycomp</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Texas Instruments</t>
   </si>
   <si>
+    <t>Microchip</t>
+  </si>
+  <si>
     <t>Manufacturer Part Number 1</t>
   </si>
   <si>
-    <t>06035C104KAT2A</t>
-  </si>
-  <si>
-    <t>GCM1885C2A220JA16D</t>
+    <t>C0603C103J5JACTU</t>
+  </si>
+  <si>
+    <t>06035C-104KAT2A</t>
   </si>
   <si>
     <t>UMK107AB7105KA-T</t>
@@ -230,10 +269,22 @@
     <t>150060VS75000</t>
   </si>
   <si>
-    <t>5600200620</t>
-  </si>
-  <si>
-    <t>5023520400</t>
+    <t>1722861302</t>
+  </si>
+  <si>
+    <t>560020-0220</t>
+  </si>
+  <si>
+    <t>560020-0620</t>
+  </si>
+  <si>
+    <t>10132797-055100LF</t>
+  </si>
+  <si>
+    <t>560020-0420</t>
+  </si>
+  <si>
+    <t>RC0603FR-074K7L</t>
   </si>
   <si>
     <t>RC0603FR-0710KL</t>
@@ -242,18 +293,15 @@
     <t>RC0603FR-07100RL</t>
   </si>
   <si>
-    <t>RC0603JR-07510RL</t>
-  </si>
-  <si>
-    <t>EM3242</t>
+    <t>OPA2197IDGKR</t>
+  </si>
+  <si>
+    <t>ADS1015IDGSR</t>
   </si>
   <si>
     <t>MIC94310-PYMT-TR</t>
   </si>
   <si>
-    <t>ADS1015IDGSR</t>
-  </si>
-  <si>
     <t>Supplier 1</t>
   </si>
   <si>
@@ -263,22 +311,34 @@
     <t>Supplier Part Number 1</t>
   </si>
   <si>
+    <t>399-13384-1-ND</t>
+  </si>
+  <si>
     <t>478-5052-1-ND</t>
   </si>
   <si>
-    <t>490-4942-1-ND</t>
-  </si>
-  <si>
     <t>587-3247-1-ND</t>
   </si>
   <si>
     <t>732-4980-1-ND</t>
   </si>
   <si>
+    <t>WM11673-ND</t>
+  </si>
+  <si>
+    <t>WM10862CT-ND</t>
+  </si>
+  <si>
     <t>WM10866CT-ND</t>
   </si>
   <si>
-    <t>WM7171CT-ND</t>
+    <t>609-5226-1-ND</t>
+  </si>
+  <si>
+    <t>WM10864CT-ND</t>
+  </si>
+  <si>
+    <t>311-4.70KHRCT-ND</t>
   </si>
   <si>
     <t>311-10.0KHRCT-ND</t>
@@ -287,18 +347,15 @@
     <t>311-100HRCT-ND</t>
   </si>
   <si>
-    <t>311-510GRCT-ND</t>
-  </si>
-  <si>
-    <t>974-1044-1-ND</t>
+    <t>296-47349-1-ND</t>
+  </si>
+  <si>
+    <t>296-41185-1-ND</t>
   </si>
   <si>
     <t>576-4761-1-ND</t>
   </si>
   <si>
-    <t>296-41185-1-ND</t>
-  </si>
-  <si>
     <t>Supplier Unit Price 1</t>
   </si>
   <si>
@@ -308,19 +365,19 @@
     <t>Supplier Subtotal 1</t>
   </si>
   <si>
-    <t>C:\Users\Beshoy\Documents\midsun\hardware\MSXII_PedalBoard\MSXII_PedalBoard.PrjPcb</t>
+    <t>C:\Users\Taiping\Documents\MidnightSun\hardware\MSXII_PedalBoard\MSXII_PedalBoard.PrjPcb</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>Bill of Materials For Project [MSXII_PedalBoard.PrjPcb] (No PCB Document Selected)</t>
-  </si>
-  <si>
-    <t>8:08:38 PM</t>
-  </si>
-  <si>
-    <t>22/05/2018</t>
+    <t>7:44:58 PM</t>
+  </si>
+  <si>
+    <t>2019-01-18</t>
+  </si>
+  <si>
+    <t>Copy of Bill of Materials</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -332,7 +389,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -578,7 +635,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE3F1136-DCE1-4A70-959E-FE57A9093CD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3F1136-DCE1-4A70-959E-FE57A9093CD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -902,38 +959,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J26"/>
+  <dimension ref="A2:J30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12" style="5" customWidth="1"/>
-    <col min="6" max="6" width="21" style="5" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="41.265625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="38.265625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.73046875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="26.19921875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.06640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.9296875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.46484375" style="5" customWidth="1"/>
     <col min="8" max="8" width="16" style="5" customWidth="1"/>
-    <col min="9" max="9" width="20" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="9" max="9" width="19.9296875" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>15</v>
       </c>
@@ -941,7 +998,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
@@ -949,7 +1006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>18</v>
       </c>
@@ -957,7 +1014,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>19</v>
       </c>
@@ -970,7 +1027,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>20</v>
       </c>
@@ -983,7 +1040,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
@@ -993,7 +1050,7 @@
       <c r="C7" s="21"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>17</v>
       </c>
@@ -1002,7 +1059,7 @@
       </c>
       <c r="C8" s="21"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>22</v>
       </c>
@@ -1011,425 +1068,529 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="G12" s="3">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="H12" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I12" s="8">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="G13" s="3">
         <v>0.17</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I13" s="8">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H14" s="3">
         <v>2</v>
       </c>
       <c r="I14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="G15" s="3">
-        <v>0.19</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
       </c>
       <c r="I15" s="8">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G16" s="3">
-        <v>1.68</v>
+        <v>1.46</v>
       </c>
       <c r="H16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="8">
-        <v>3.36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="G17" s="3">
-        <v>1.9</v>
+        <v>0.78</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
       </c>
       <c r="I17" s="8">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="G18" s="3">
-        <v>0.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
       </c>
       <c r="I18" s="8">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="29" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="H19" s="3">
-        <v>2</v>
-      </c>
-      <c r="I19" s="8">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="29" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="G20" s="3">
-        <v>0.15</v>
+        <v>1.66</v>
       </c>
       <c r="H20" s="3">
         <v>1</v>
       </c>
       <c r="I20" s="8">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="G21" s="3">
-        <v>7.08</v>
+        <v>0.1</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I21" s="8">
-        <v>7.08</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="29" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="G22" s="3">
-        <v>0.43</v>
+        <v>0.1</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="8">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F23" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="3">
-        <v>4.08</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="F24" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>4</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2.41</v>
+      </c>
+      <c r="H25" s="3">
+        <v>2</v>
+      </c>
+      <c r="I25" s="8">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="H26" s="3">
         <v>1</v>
       </c>
-      <c r="I23" s="8">
-        <v>4.08</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="3" t="s">
+      <c r="I26" s="8">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="12">
-        <f>SUM(I12:I23)</f>
-        <v>18.47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="15"/>
+      <c r="I28" s="12">
+        <f>SUM(I12:I27)</f>
+        <v>18.03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1437,76 +1598,88 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" tooltip="Component" display="'AVX Corporation"/>
-    <hyperlink ref="C13" r:id="rId2" tooltip="Component" display="'Murata Electronics North America"/>
-    <hyperlink ref="C14" r:id="rId3" tooltip="Component" display="'Taiyo Yuden"/>
-    <hyperlink ref="C15" r:id="rId4" tooltip="Component" display="'Wurth Electronics Inc."/>
-    <hyperlink ref="C16" r:id="rId5" tooltip="Component" display="'Molex, LLC"/>
-    <hyperlink ref="C17" r:id="rId6" tooltip="Component" display="'Molex, LLC"/>
-    <hyperlink ref="C18" r:id="rId7" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="C19" r:id="rId8" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="C20" r:id="rId9" tooltip="Component" display="'Yageo"/>
-    <hyperlink ref="C21" r:id="rId10" tooltip="Component" display="'AKM Semiconductor Inc."/>
-    <hyperlink ref="C22" r:id="rId11" tooltip="Component" display="'Microchip Technology"/>
-    <hyperlink ref="C23" r:id="rId12" tooltip="Component" display="'Texas Instruments"/>
-    <hyperlink ref="D12" r:id="rId13" tooltip="Manufacturer" display="'06035C104KAT2A"/>
-    <hyperlink ref="D13" r:id="rId14" tooltip="Manufacturer" display="'GCM1885C2A220JA16D"/>
-    <hyperlink ref="D14" r:id="rId15" tooltip="Manufacturer" display="'UMK107AB7105KA-T"/>
-    <hyperlink ref="D15" r:id="rId16" tooltip="Manufacturer" display="'150060VS75000"/>
-    <hyperlink ref="D16" r:id="rId17" tooltip="Manufacturer" display="'5600200620"/>
-    <hyperlink ref="D17" r:id="rId18" tooltip="Manufacturer" display="'5023520400"/>
-    <hyperlink ref="D18" r:id="rId19" tooltip="Manufacturer" display="'RC0603FR-0710KL"/>
-    <hyperlink ref="D19" r:id="rId20" tooltip="Manufacturer" display="'RC0603FR-07100RL"/>
-    <hyperlink ref="D20" r:id="rId21" tooltip="Manufacturer" display="'RC0603JR-07510RL"/>
-    <hyperlink ref="D21" r:id="rId22" tooltip="Manufacturer" display="'EM3242"/>
-    <hyperlink ref="D22" r:id="rId23" tooltip="Manufacturer" display="'MIC94310-PYMT-TR"/>
-    <hyperlink ref="D23" r:id="rId24" tooltip="Manufacturer" display="'ADS1015IDGSR"/>
-    <hyperlink ref="F12" r:id="rId25" tooltip="Supplier" display="'478-5052-1-ND"/>
-    <hyperlink ref="F13" r:id="rId26" tooltip="Supplier" display="'490-4942-1-ND"/>
-    <hyperlink ref="F14" r:id="rId27" tooltip="Supplier" display="'587-3247-1-ND"/>
-    <hyperlink ref="F15" r:id="rId28" tooltip="Supplier" display="'732-4980-1-ND"/>
-    <hyperlink ref="F16" r:id="rId29" tooltip="Supplier" display="'WM10866CT-ND"/>
-    <hyperlink ref="F17" r:id="rId30" tooltip="Supplier" display="'WM7171CT-ND"/>
-    <hyperlink ref="F18" r:id="rId31" tooltip="Supplier" display="'311-10.0KHRCT-ND"/>
-    <hyperlink ref="F19" r:id="rId32" tooltip="Supplier" display="'311-100HRCT-ND"/>
-    <hyperlink ref="F20" r:id="rId33" tooltip="Supplier" display="'311-510GRCT-ND"/>
-    <hyperlink ref="F21" r:id="rId34" tooltip="Supplier" display="'974-1044-1-ND"/>
-    <hyperlink ref="F22" r:id="rId35" tooltip="Supplier" display="'576-4761-1-ND"/>
-    <hyperlink ref="F23" r:id="rId36" tooltip="Supplier" display="'296-41185-1-ND"/>
+    <hyperlink ref="C12" r:id="rId1" tooltip="Component" display="'KEMET" xr:uid="{876F45A7-8436-4AD6-A3A2-4EC9147FFB39}"/>
+    <hyperlink ref="C13" r:id="rId2" tooltip="Component" display="'Kyocera AVX" xr:uid="{AD35F2A4-990E-453D-AEDD-AF7C24610530}"/>
+    <hyperlink ref="C14" r:id="rId3" tooltip="Component" display="'Taiyo Yuden" xr:uid="{8BD60DDC-B5C5-4B16-92C4-3B868A062F40}"/>
+    <hyperlink ref="C15" r:id="rId4" tooltip="Component" display="'Wurth Electronics" xr:uid="{63CB6FB2-0B8A-4435-945A-7C6E5806CD05}"/>
+    <hyperlink ref="C16" r:id="rId5" tooltip="Component" display="'Molex" xr:uid="{563FB109-BBD1-4175-B5FC-AD80208C18DC}"/>
+    <hyperlink ref="C17" r:id="rId6" tooltip="Component" display="'Molex" xr:uid="{F9902253-06A8-4918-8FF7-8B7A5390B530}"/>
+    <hyperlink ref="C18" r:id="rId7" tooltip="Component" display="'Molex" xr:uid="{12C89596-049D-4CB0-949C-8DA6A31B3533}"/>
+    <hyperlink ref="C19" r:id="rId8" tooltip="Component" display="'Amphenol FCI" xr:uid="{17535025-1FE6-4B0E-AB5A-1CB4562F7676}"/>
+    <hyperlink ref="C20" r:id="rId9" tooltip="Component" display="'Molex" xr:uid="{3F6C3A30-630E-4B84-A106-14F8617F6264}"/>
+    <hyperlink ref="C21" r:id="rId10" tooltip="Component" display="'Yageo" xr:uid="{EEBA1F0B-EB04-4A99-8ACB-524BD779B9D0}"/>
+    <hyperlink ref="C22" r:id="rId11" tooltip="Component" display="'Yageo Phycomp" xr:uid="{A69E3D09-8E0B-419E-8D03-CA1C1351503A}"/>
+    <hyperlink ref="C23" tooltip="Component" display="'" xr:uid="{4C388B89-EC85-4EF5-BCD5-0AF023100684}"/>
+    <hyperlink ref="C24" r:id="rId12" tooltip="Component" display="'Yageo" xr:uid="{4FD81D38-E1F9-41BB-AF50-E17AE82F8058}"/>
+    <hyperlink ref="C25" r:id="rId13" tooltip="Component" display="'Texas Instruments" xr:uid="{DBA88CED-0CEF-4947-ABEF-870262593094}"/>
+    <hyperlink ref="C26" r:id="rId14" tooltip="Component" display="'Texas Instruments" xr:uid="{8C243454-391B-4C9D-9A02-0CFA64545F7F}"/>
+    <hyperlink ref="C27" r:id="rId15" tooltip="Component" display="'Microchip" xr:uid="{F0B40537-5B8E-47C6-B9CD-13EEFCCD3787}"/>
+    <hyperlink ref="D12" r:id="rId16" tooltip="Manufacturer" display="'C0603C103J5JACTU" xr:uid="{7B124A50-DA9F-469C-B1B7-D85B5E0E3F1B}"/>
+    <hyperlink ref="D13" r:id="rId17" tooltip="Manufacturer" display="'06035C-104KAT2A" xr:uid="{520CA853-E3AB-4523-A17D-959FB52D8339}"/>
+    <hyperlink ref="D14" r:id="rId18" tooltip="Manufacturer" display="'UMK107AB7105KA-T" xr:uid="{A2477B35-7EDA-4483-875A-46DEBAB1ED67}"/>
+    <hyperlink ref="D15" r:id="rId19" tooltip="Manufacturer" display="'150060VS75000" xr:uid="{0D9F0D39-D0A5-49A5-B844-2EFEEE214FD2}"/>
+    <hyperlink ref="D16" r:id="rId20" tooltip="Manufacturer" display="'1722861302" xr:uid="{7D2A8E73-8DB3-4719-8D3C-390D9AAD6785}"/>
+    <hyperlink ref="D17" r:id="rId21" tooltip="Manufacturer" display="'560020-0220" xr:uid="{318FEDDE-E09D-4CF2-B815-EDBC3F73F042}"/>
+    <hyperlink ref="D18" r:id="rId22" tooltip="Manufacturer" display="'560020-0620" xr:uid="{A4C664AD-A5C0-4E24-8C1E-ADE3B0C76ED1}"/>
+    <hyperlink ref="D19" r:id="rId23" tooltip="Manufacturer" display="'10132797-055100LF" xr:uid="{E6788146-3E4C-4C45-84B6-8267C55EAE2F}"/>
+    <hyperlink ref="D20" r:id="rId24" tooltip="Manufacturer" display="'560020-0420" xr:uid="{CEE65E38-89BC-4E65-950F-61FBD5BD1CF6}"/>
+    <hyperlink ref="D21" r:id="rId25" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{A89131EF-C6D6-41A2-A73B-5709FFA4352E}"/>
+    <hyperlink ref="D22" r:id="rId26" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{826B86C3-7B65-41C0-B423-BED4A051538B}"/>
+    <hyperlink ref="D23" tooltip="Manufacturer" display="'" xr:uid="{F7B8BF1A-0710-4FF3-BC0D-4A561582F678}"/>
+    <hyperlink ref="D24" r:id="rId27" tooltip="Manufacturer" display="'RC0603FR-07100RL" xr:uid="{856A8732-5F79-4921-BFE2-FA1EA4C92548}"/>
+    <hyperlink ref="D25" r:id="rId28" tooltip="Manufacturer" display="'OPA2197IDGKR" xr:uid="{A2C0E2AE-5F21-4767-9166-E1004F8C727B}"/>
+    <hyperlink ref="D26" r:id="rId29" tooltip="Manufacturer" display="'ADS1015IDGSR" xr:uid="{9A97C895-DD1F-4689-87A4-B08A85D86842}"/>
+    <hyperlink ref="D27" r:id="rId30" tooltip="Manufacturer" display="'MIC94310-PYMT-TR" xr:uid="{25D7B950-37F4-4F0F-8DE9-455A7663EED7}"/>
+    <hyperlink ref="F12" r:id="rId31" tooltip="Supplier" display="'399-13384-1-ND" xr:uid="{58697948-537F-4248-A877-5DAB65B025F0}"/>
+    <hyperlink ref="F13" r:id="rId32" tooltip="Supplier" display="'478-5052-1-ND" xr:uid="{168EDDE6-75CE-489D-B6E2-A3967640A18D}"/>
+    <hyperlink ref="F14" r:id="rId33" tooltip="Supplier" display="'587-3247-1-ND" xr:uid="{5E33D966-0CF9-428F-ABFF-F8D9F0514838}"/>
+    <hyperlink ref="F15" r:id="rId34" tooltip="Supplier" display="'732-4980-1-ND" xr:uid="{0EECAC69-CFBE-4F9E-BD08-827888CE9C65}"/>
+    <hyperlink ref="F16" r:id="rId35" tooltip="Supplier" display="'WM11673-ND" xr:uid="{2AF12AA5-5633-47AA-8D4C-C3A9000C420A}"/>
+    <hyperlink ref="F17" r:id="rId36" tooltip="Supplier" display="'WM10862CT-ND" xr:uid="{79AA81C4-E5D4-4D57-B736-427E309F2CD9}"/>
+    <hyperlink ref="F18" r:id="rId37" tooltip="Supplier" display="'WM10866CT-ND" xr:uid="{EE9237A5-EF35-40BF-A003-C1E078FC2A60}"/>
+    <hyperlink ref="F19" r:id="rId38" tooltip="Supplier" display="'609-5226-1-ND" xr:uid="{59632A4B-1E83-448D-A595-85AAA0219F99}"/>
+    <hyperlink ref="F20" r:id="rId39" tooltip="Supplier" display="'WM10864CT-ND" xr:uid="{3F30B313-E29F-4FE4-BA03-8997737CB983}"/>
+    <hyperlink ref="F21" r:id="rId40" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{6D0FB029-76B7-4DD7-B919-0488B9EA867F}"/>
+    <hyperlink ref="F22" r:id="rId41" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{CF88AA1E-B685-4CCF-9EEF-9A3268D6758E}"/>
+    <hyperlink ref="F23" tooltip="Supplier" display="'" xr:uid="{33365950-5615-45C6-A075-461CE0BC6FE4}"/>
+    <hyperlink ref="F24" r:id="rId42" tooltip="Supplier" display="'311-100HRCT-ND" xr:uid="{104BDEC5-34BD-4D20-903E-2D21AA9E24BA}"/>
+    <hyperlink ref="F25" r:id="rId43" tooltip="Supplier" display="'296-47349-1-ND" xr:uid="{7FF9615A-BC61-4737-B847-BF62C05B8E49}"/>
+    <hyperlink ref="F26" r:id="rId44" tooltip="Supplier" display="'296-41185-1-ND" xr:uid="{01BE4EBF-1AAB-43D1-A35F-7DE4E1BE0795}"/>
+    <hyperlink ref="F27" r:id="rId45" tooltip="Supplier" display="'576-4761-1-ND" xr:uid="{62D3BD52-76F8-400A-A25E-D422A087B629}"/>
   </hyperlinks>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId37"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId46"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;BAltium Limited Confidential&amp;B&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId38"/>
+  <drawing r:id="rId47"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="A1:IV65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="108.5703125" style="17" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="30.265625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="108.59765625" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
@@ -1514,15 +1687,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
@@ -1530,23 +1703,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
@@ -1554,23 +1727,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>10</v>
       </c>
@@ -1578,31 +1751,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>13</v>
       </c>

</xml_diff>